<commit_message>
update progress in gantt chart
</commit_message>
<xml_diff>
--- a/Documentation/Gantt_Chart_Template.xlsx
+++ b/Documentation/Gantt_Chart_Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{3E30FD7B-FE22-41C1-8AE7-A8B1DE8F1B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC874CB0-B546-4C0E-9634-2AF37DC3F244}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{3E30FD7B-FE22-41C1-8AE7-A8B1DE8F1B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63E957E6-3564-4D97-A327-7A51C84BD05B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,28 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
-  <si>
-    <t>Phase 1 Title</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Phase 2 Title</t>
-  </si>
-  <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -75,9 +54,6 @@
 TO</t>
   </si>
   <si>
-    <t>PROJECT TITLE</t>
-  </si>
-  <si>
     <t>Project Management Templates</t>
   </si>
   <si>
@@ -96,9 +72,6 @@
     <t>TASK</t>
   </si>
   <si>
-    <t>Phase 3 Title</t>
-  </si>
-  <si>
     <t>More Project Management Templates</t>
   </si>
   <si>
@@ -132,16 +105,7 @@
     <t>This template provides a simple way to create a Gantt chart to help visualize and track your project. Simply enter your tasks and start and end dates - no formulas required. The bars in the Gantt chart represent the duration of the task and are displayed using conditional formatting. Insert new tasks by inserting new rows.</t>
   </si>
   <si>
-    <t>Phase 4 Title</t>
-  </si>
-  <si>
     <t>Click on the link below to visit vertex42.com and learn more about how to use this template, such as how to calculate days and work days, create task dependencies, change the colors of the bars, add a scroll bar to make it easier to change the display week, extend the date range displayed in the chart, etc.</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Project Lead</t>
   </si>
   <si>
     <t>There are 2 worksheets in this workbook. 
@@ -156,12 +120,6 @@
   </si>
   <si>
     <t>Enter Company Name in cell B2.</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>Sample phase title block</t>
@@ -235,6 +193,72 @@
 Continue navigating down column A cells to learn more.
 If you haven't added any new rows in this worksheet, you will find 2 additional sample phase blocks have been created for you in cells B20 and B26. Otherwise, navigate through column A cells to find the additional blocks. 
 Repeat the instructions from cells A8 and A9 whenever you need to.</t>
+  </si>
+  <si>
+    <t>Devolpement Planning</t>
+  </si>
+  <si>
+    <t>Daniyal &amp; Saket</t>
+  </si>
+  <si>
+    <t>Setting up github</t>
+  </si>
+  <si>
+    <t>Project Planning</t>
+  </si>
+  <si>
+    <t>Finish up project planning</t>
+  </si>
+  <si>
+    <t>Daniyal</t>
+  </si>
+  <si>
+    <t>Coding/Github</t>
+  </si>
+  <si>
+    <t>Coding/Documentation</t>
+  </si>
+  <si>
+    <t>Final Coding/Presentation</t>
+  </si>
+  <si>
+    <t>Create Basic GUI</t>
+  </si>
+  <si>
+    <t>Create Profile</t>
+  </si>
+  <si>
+    <t>Create Calcalutor</t>
+  </si>
+  <si>
+    <t>Finalize GUI</t>
+  </si>
+  <si>
+    <t>Work on Calcalutor</t>
+  </si>
+  <si>
+    <t>Finalize Code</t>
+  </si>
+  <si>
+    <t>Work on Documentation</t>
+  </si>
+  <si>
+    <t>Push Code &amp; Documentation</t>
+  </si>
+  <si>
+    <t>Work on Code</t>
+  </si>
+  <si>
+    <t>Student Dev Team</t>
+  </si>
+  <si>
+    <t>Money Management Application</t>
+  </si>
+  <si>
+    <t>(Possiable Extention Time)</t>
+  </si>
+  <si>
+    <t>Present Project</t>
   </si>
 </sst>
 </file>
@@ -248,7 +272,7 @@
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +433,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -645,7 +676,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -887,6 +918,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -894,17 +937,8 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1206,6 +1240,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1476,7 +1514,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1495,10 +1533,10 @@
   <sheetData>
     <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="59" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1506,138 +1544,138 @@
       <c r="F1" s="47"/>
       <c r="H1" s="2"/>
       <c r="I1" s="14" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="58" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B2" s="64" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="I2" s="61" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="58" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="85" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="91">
+        <v>39</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="90"/>
+      <c r="E3" s="88">
         <v>45788</v>
       </c>
-      <c r="F3" s="91"/>
+      <c r="F3" s="88"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="86"/>
+        <v>31</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="90"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="88">
+      <c r="I4" s="85">
         <f>I5</f>
         <v>45789</v>
       </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="88">
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="85">
         <f>P5</f>
         <v>45796</v>
       </c>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="88">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="85">
         <f>W5</f>
         <v>45803</v>
       </c>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="88">
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87"/>
+      <c r="AD4" s="85">
         <f>AD5</f>
         <v>45810</v>
       </c>
-      <c r="AE4" s="89"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="88">
+      <c r="AE4" s="86"/>
+      <c r="AF4" s="86"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="86"/>
+      <c r="AJ4" s="87"/>
+      <c r="AK4" s="85">
         <f>AK5</f>
         <v>45817</v>
       </c>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="88">
+      <c r="AL4" s="86"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="86"/>
+      <c r="AO4" s="86"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="87"/>
+      <c r="AR4" s="85">
         <f>AR5</f>
         <v>45824</v>
       </c>
-      <c r="AS4" s="89"/>
-      <c r="AT4" s="89"/>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="88">
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="86"/>
+      <c r="AU4" s="86"/>
+      <c r="AV4" s="86"/>
+      <c r="AW4" s="86"/>
+      <c r="AX4" s="87"/>
+      <c r="AY4" s="85">
         <f>AY5</f>
         <v>45831</v>
       </c>
-      <c r="AZ4" s="89"/>
-      <c r="BA4" s="89"/>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="88">
+      <c r="AZ4" s="86"/>
+      <c r="BA4" s="86"/>
+      <c r="BB4" s="86"/>
+      <c r="BC4" s="86"/>
+      <c r="BD4" s="86"/>
+      <c r="BE4" s="87"/>
+      <c r="BF4" s="85">
         <f>BF5</f>
         <v>45838</v>
       </c>
-      <c r="BG4" s="89"/>
-      <c r="BH4" s="89"/>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="90"/>
+      <c r="BG4" s="86"/>
+      <c r="BH4" s="86"/>
+      <c r="BI4" s="86"/>
+      <c r="BJ4" s="86"/>
+      <c r="BK4" s="86"/>
+      <c r="BL4" s="87"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
+        <v>32</v>
+      </c>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>45789</v>
@@ -1865,26 +1903,26 @@
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="59" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="I6" s="13" t="str">
         <f t="shared" ref="I6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -2113,7 +2151,7 @@
     </row>
     <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="58" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C7" s="62"/>
       <c r="E7"/>
@@ -2180,10 +2218,10 @@
     </row>
     <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="59" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C8" s="71"/>
       <c r="D8" s="19"/>
@@ -2253,16 +2291,16 @@
     </row>
     <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="59" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C9" s="72" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="22">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="66">
         <f>Project_Start</f>
@@ -2336,14 +2374,16 @@
     </row>
     <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="59" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B10" s="80" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="72"/>
+        <v>40</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>39</v>
+      </c>
       <c r="D10" s="22">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E10" s="66">
         <f>F9</f>
@@ -2418,11 +2458,13 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="58"/>
       <c r="B11" s="80" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="22">
         <v>1</v>
-      </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="22">
-        <v>0.5</v>
       </c>
       <c r="E11" s="66">
         <f>F10</f>
@@ -2497,11 +2539,13 @@
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="58"/>
       <c r="B12" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="72"/>
+        <v>41</v>
+      </c>
+      <c r="C12" s="72" t="s">
+        <v>39</v>
+      </c>
       <c r="D12" s="22">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="E12" s="66">
         <f>F11</f>
@@ -2576,10 +2620,14 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="58"/>
       <c r="B13" s="80" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="22"/>
+        <v>42</v>
+      </c>
+      <c r="C13" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
       <c r="E13" s="66">
         <f>E10+1</f>
         <v>45792</v>
@@ -2652,10 +2700,10 @@
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="59" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C14" s="73"/>
       <c r="D14" s="24"/>
@@ -2726,11 +2774,13 @@
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="59"/>
       <c r="B15" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="74"/>
+        <v>47</v>
+      </c>
+      <c r="C15" s="74" t="s">
+        <v>43</v>
+      </c>
       <c r="D15" s="27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="67">
         <f>E13+1</f>
@@ -2805,11 +2855,13 @@
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="58"/>
       <c r="B16" s="81" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="74"/>
+        <v>47</v>
+      </c>
+      <c r="C16" s="74" t="s">
+        <v>43</v>
+      </c>
       <c r="D16" s="27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E16" s="67">
         <f>E15+2</f>
@@ -2884,10 +2936,14 @@
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="58"/>
       <c r="B17" s="81" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="27">
         <v>1</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="27"/>
       <c r="E17" s="67">
         <f>F16</f>
         <v>45800</v>
@@ -2961,10 +3017,14 @@
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="58"/>
       <c r="B18" s="81" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="74"/>
-      <c r="D18" s="27"/>
+        <v>49</v>
+      </c>
+      <c r="C18" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="27">
+        <v>1</v>
+      </c>
       <c r="E18" s="67">
         <f>E17</f>
         <v>45800</v>
@@ -3038,10 +3098,14 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="58"/>
       <c r="B19" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="74"/>
-      <c r="D19" s="27"/>
+        <v>50</v>
+      </c>
+      <c r="C19" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="27">
+        <v>0.6</v>
+      </c>
       <c r="E19" s="67">
         <f>E18</f>
         <v>45800</v>
@@ -3114,10 +3178,10 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="58" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="C20" s="75"/>
       <c r="D20" s="29"/>
@@ -3188,10 +3252,14 @@
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="58"/>
       <c r="B21" s="82" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="32"/>
+        <v>51</v>
+      </c>
+      <c r="C21" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="32">
+        <v>1</v>
+      </c>
       <c r="E21" s="68">
         <f>E9+15</f>
         <v>45803</v>
@@ -3265,10 +3333,14 @@
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="58"/>
       <c r="B22" s="82" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="76"/>
-      <c r="D22" s="32"/>
+        <v>53</v>
+      </c>
+      <c r="C22" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="32">
+        <v>0.5</v>
+      </c>
       <c r="E22" s="68">
         <f>F21+1</f>
         <v>45809</v>
@@ -3342,22 +3414,25 @@
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="58"/>
       <c r="B23" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="32"/>
+        <v>53</v>
+      </c>
+      <c r="C23" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="32">
+        <v>0.5</v>
+      </c>
       <c r="E23" s="68">
         <f>E22+5</f>
         <v>45814</v>
       </c>
       <c r="F23" s="68">
-        <f>E23+5</f>
-        <v>45819</v>
+        <v>45817</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I23" s="44"/>
       <c r="J23" s="44"/>
@@ -3419,22 +3494,25 @@
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="58"/>
       <c r="B24" s="82" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="76"/>
-      <c r="D24" s="32"/>
+        <v>54</v>
+      </c>
+      <c r="C24" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="32">
+        <v>0.98</v>
+      </c>
       <c r="E24" s="68">
         <f>F23+1</f>
+        <v>45818</v>
+      </c>
+      <c r="F24" s="68">
         <v>45820</v>
-      </c>
-      <c r="F24" s="68">
-        <f>E24+4</f>
-        <v>45824</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I24" s="44"/>
       <c r="J24" s="44"/>
@@ -3496,22 +3574,24 @@
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="58"/>
       <c r="B25" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="32"/>
+        <v>55</v>
+      </c>
+      <c r="C25" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="32">
+        <v>0.75</v>
+      </c>
       <c r="E25" s="68">
-        <f>E23</f>
-        <v>45814</v>
+        <v>45821</v>
       </c>
       <c r="F25" s="68">
-        <f>E25+4</f>
-        <v>45818</v>
+        <v>45823</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I25" s="44"/>
       <c r="J25" s="44"/>
@@ -3572,10 +3652,10 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="58" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C26" s="77"/>
       <c r="D26" s="34"/>
@@ -3646,20 +3726,24 @@
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="58"/>
       <c r="B27" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="78"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="69" t="s">
-        <v>37</v>
+        <v>52</v>
+      </c>
+      <c r="C27" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="37">
+        <v>0</v>
+      </c>
+      <c r="E27" s="69">
+        <v>45823</v>
+      </c>
+      <c r="F27" s="69">
+        <v>45824</v>
       </c>
       <c r="G27" s="17"/>
-      <c r="H27" s="17" t="e">
+      <c r="H27" s="17">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>2</v>
       </c>
       <c r="I27" s="44"/>
       <c r="J27" s="44"/>
@@ -3721,20 +3805,24 @@
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="58"/>
       <c r="B28" s="83" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="78"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="69" t="s">
-        <v>37</v>
+        <v>59</v>
+      </c>
+      <c r="C28" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="37">
+        <v>0</v>
+      </c>
+      <c r="E28" s="69">
+        <v>45825</v>
+      </c>
+      <c r="F28" s="69">
+        <v>45825</v>
       </c>
       <c r="G28" s="17"/>
-      <c r="H28" s="17" t="e">
+      <c r="H28" s="17">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="I28" s="44"/>
       <c r="J28" s="44"/>
@@ -3795,21 +3883,23 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="58"/>
-      <c r="B29" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="78"/>
+      <c r="B29" s="92" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="78" t="s">
+        <v>43</v>
+      </c>
       <c r="D29" s="37"/>
-      <c r="E29" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="69" t="s">
-        <v>37</v>
+      <c r="E29" s="69">
+        <v>45826</v>
+      </c>
+      <c r="F29" s="69">
+        <v>45827</v>
       </c>
       <c r="G29" s="17"/>
-      <c r="H29" s="17" t="e">
+      <c r="H29" s="17">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>2</v>
       </c>
       <c r="I29" s="44"/>
       <c r="J29" s="44"/>
@@ -3870,21 +3960,23 @@
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="58"/>
-      <c r="B30" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="78"/>
+      <c r="B30" s="92" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="78" t="s">
+        <v>43</v>
+      </c>
       <c r="D30" s="37"/>
-      <c r="E30" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="F30" s="69" t="s">
-        <v>37</v>
+      <c r="E30" s="69">
+        <v>45828</v>
+      </c>
+      <c r="F30" s="69">
+        <v>45828</v>
       </c>
       <c r="G30" s="17"/>
-      <c r="H30" s="17" t="e">
+      <c r="H30" s="17">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="I30" s="44"/>
       <c r="J30" s="44"/>
@@ -3945,21 +4037,23 @@
     </row>
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="58"/>
-      <c r="B31" s="83" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="78"/>
+      <c r="B31" s="92" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="78" t="s">
+        <v>43</v>
+      </c>
       <c r="D31" s="37"/>
-      <c r="E31" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="69" t="s">
-        <v>37</v>
+      <c r="E31" s="69">
+        <v>45829</v>
+      </c>
+      <c r="F31" s="69">
+        <v>45829</v>
       </c>
       <c r="G31" s="17"/>
-      <c r="H31" s="17" t="e">
+      <c r="H31" s="17">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="I31" s="44"/>
       <c r="J31" s="44"/>
@@ -4020,7 +4114,7 @@
     </row>
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="58" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B32" s="84"/>
       <c r="C32" s="79"/>
@@ -4091,10 +4185,10 @@
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="59" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C33" s="39"/>
       <c r="D33" s="40"/>
@@ -4174,6 +4268,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4181,11 +4280,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">
@@ -4230,7 +4324,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F18 F22:F23 E23" formula="1"/>
+    <ignoredError sqref="F18 F22 E23" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4260,7 +4354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4271,79 +4365,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" s="50" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="49" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B2" s="49"/>
     </row>
     <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="55" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B3" s="55"/>
     </row>
     <row r="4" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A4" s="52" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="53" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="52" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="48" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="57" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A8" s="52" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.3">
       <c r="A9" s="53" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="48" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="56" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A11" s="52" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.3">
       <c r="A12" s="53" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="48" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="56" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A14" s="52" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="53" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A16" s="53" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -4360,6 +4454,70 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Has_Teacher_Only_SectionGroup xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <FolderType xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TeamsChannelId xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <Invited_Teachers xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <Invited_Students xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <Templates xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <Teachers xmlns="147d1278-e733-49aa-b400-ef7687d76ce3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Distribution_Groups xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <LMS_Mappings xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <CultureName xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <AppVersion xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <NotebookType xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <Student_Groups xmlns="147d1278-e733-49aa-b400-ef7687d76ce3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Math_Settings xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <Owner xmlns="147d1278-e733-49aa-b400-ef7687d76ce3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Students xmlns="147d1278-e733-49aa-b400-ef7687d76ce3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Is_Collaboration_Space_Locked xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+    <_activity xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A6C24D38A47D4483BDD40956192BCF" ma:contentTypeVersion="39" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f07f3829e5d09499baf2c8502db3ed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="147d1278-e733-49aa-b400-ef7687d76ce3" xmlns:ns4="93d03e77-3551-4536-9208-3222abea9772" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae3c4703f3b8d4021d69f44788502e31" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4811,71 +4969,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4166818-70F8-4D06-AC57-4B3E04A31479}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="93d03e77-3551-4536-9208-3222abea9772"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="147d1278-e733-49aa-b400-ef7687d76ce3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Has_Teacher_Only_SectionGroup xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <FolderType xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TeamsChannelId xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <Invited_Teachers xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <Invited_Students xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <Templates xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <Teachers xmlns="147d1278-e733-49aa-b400-ef7687d76ce3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Distribution_Groups xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <LMS_Mappings xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <CultureName xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <AppVersion xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <NotebookType xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <Student_Groups xmlns="147d1278-e733-49aa-b400-ef7687d76ce3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Math_Settings xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <Owner xmlns="147d1278-e733-49aa-b400-ef7687d76ce3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Students xmlns="147d1278-e733-49aa-b400-ef7687d76ce3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Is_Collaboration_Space_Locked xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-    <_activity xmlns="147d1278-e733-49aa-b400-ef7687d76ce3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02FA432F-35E5-44AC-838D-D2937AF03E34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E51B8CD0-936E-4F4B-BD26-D0FCA6E1F434}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4893,30 +5013,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02FA432F-35E5-44AC-838D-D2937AF03E34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4166818-70F8-4D06-AC57-4B3E04A31479}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="93d03e77-3551-4536-9208-3222abea9772"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="147d1278-e733-49aa-b400-ef7687d76ce3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>